<commit_message>
Update Data in Sheet
</commit_message>
<xml_diff>
--- a/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD.xlsx
+++ b/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Hub Latest Project\mratdd\cukesatdd\src\main\resources\database\PlanDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF7CEE3-AB64-495B-9461-D74F811FC99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8EA350-0758-46AD-9E2B-129462DCA029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="19180" windowHeight="10170" tabRatio="670" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
   </bookViews>
   <sheets>
     <sheet name="MAPD_SNP_DCE" sheetId="1" r:id="rId1"/>
@@ -8578,7 +8578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8651,6 +8651,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8970,8 +8973,8 @@
   <dimension ref="A1:Y497"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10213,6 +10216,8 @@
       <c r="R16" s="23">
         <v>131</v>
       </c>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
       <c r="U16" s="24">
         <v>100</v>
       </c>
@@ -10284,6 +10289,8 @@
       <c r="R17" s="23">
         <v>131</v>
       </c>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
       <c r="U17" s="24">
         <v>100</v>
       </c>
@@ -10355,6 +10362,8 @@
       <c r="R18" s="23">
         <v>131</v>
       </c>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
       <c r="U18" s="24">
         <v>100</v>
       </c>
@@ -10426,6 +10435,8 @@
       <c r="R19" s="23">
         <v>131</v>
       </c>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
       <c r="U19" s="24">
         <v>100</v>
       </c>
@@ -10497,6 +10508,8 @@
       <c r="R20" s="23">
         <v>131</v>
       </c>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
       <c r="U20" s="24">
         <v>100</v>
       </c>
@@ -10568,6 +10581,8 @@
       <c r="R21" s="23">
         <v>131</v>
       </c>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
       <c r="U21" s="24">
         <v>100</v>
       </c>
@@ -10639,6 +10654,8 @@
       <c r="R22" s="23">
         <v>131</v>
       </c>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
       <c r="U22" s="24">
         <v>100</v>
       </c>
@@ -10710,6 +10727,8 @@
       <c r="R23" s="23">
         <v>131</v>
       </c>
+      <c r="S23" s="30"/>
+      <c r="T23" s="30"/>
       <c r="U23" s="24">
         <v>100</v>
       </c>
@@ -10781,6 +10800,8 @@
       <c r="R24" s="23">
         <v>131</v>
       </c>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
       <c r="U24" s="24">
         <v>100</v>
       </c>
@@ -10852,6 +10873,8 @@
       <c r="R25" s="23">
         <v>131</v>
       </c>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
       <c r="U25" s="24">
         <v>100</v>
       </c>
@@ -10923,6 +10946,8 @@
       <c r="R26" s="23">
         <v>131</v>
       </c>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
       <c r="U26" s="24">
         <v>100</v>
       </c>
@@ -10994,6 +11019,8 @@
       <c r="R27" s="23">
         <v>131</v>
       </c>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
       <c r="U27" s="24">
         <v>100</v>
       </c>
@@ -11065,6 +11092,8 @@
       <c r="R28" s="23">
         <v>125</v>
       </c>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
       <c r="U28" s="24">
         <v>100</v>
       </c>
@@ -11136,6 +11165,8 @@
       <c r="R29" s="23">
         <v>131</v>
       </c>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
       <c r="U29" s="24">
         <v>100</v>
       </c>
@@ -11207,6 +11238,8 @@
       <c r="R30" s="23">
         <v>131</v>
       </c>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
       <c r="U30" s="24">
         <v>100</v>
       </c>
@@ -11278,6 +11311,8 @@
       <c r="R31" s="23">
         <v>131</v>
       </c>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
       <c r="U31" s="24">
         <v>100</v>
       </c>
@@ -11349,6 +11384,8 @@
       <c r="R32" s="23">
         <v>131</v>
       </c>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
       <c r="U32" s="24">
         <v>100</v>
       </c>
@@ -11420,6 +11457,8 @@
       <c r="R33" s="23">
         <v>131</v>
       </c>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
       <c r="U33" s="24">
         <v>100</v>
       </c>
@@ -11491,6 +11530,8 @@
       <c r="R34" s="23">
         <v>131</v>
       </c>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
       <c r="U34" s="24">
         <v>100</v>
       </c>
@@ -11562,6 +11603,8 @@
       <c r="R35" s="23">
         <v>131</v>
       </c>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
       <c r="U35" s="24">
         <v>100</v>
       </c>
@@ -11633,6 +11676,8 @@
       <c r="R36" s="23">
         <v>95</v>
       </c>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
       <c r="U36" s="24">
         <v>100</v>
       </c>
@@ -11704,6 +11749,8 @@
       <c r="R37" s="23">
         <v>131</v>
       </c>
+      <c r="S37" s="30"/>
+      <c r="T37" s="30"/>
       <c r="U37" s="24">
         <v>100</v>
       </c>
@@ -11775,6 +11822,8 @@
       <c r="R38" s="23">
         <v>131</v>
       </c>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30"/>
       <c r="U38" s="24">
         <v>100</v>
       </c>
@@ -11846,6 +11895,8 @@
       <c r="R39" s="23">
         <v>131</v>
       </c>
+      <c r="S39" s="30"/>
+      <c r="T39" s="30"/>
       <c r="U39" s="24">
         <v>100</v>
       </c>
@@ -11917,6 +11968,8 @@
       <c r="R40" s="23">
         <v>131</v>
       </c>
+      <c r="S40" s="30"/>
+      <c r="T40" s="30"/>
       <c r="U40" s="24">
         <v>100</v>
       </c>
@@ -11988,6 +12041,8 @@
       <c r="R41" s="23">
         <v>131</v>
       </c>
+      <c r="S41" s="30"/>
+      <c r="T41" s="30"/>
       <c r="U41" s="24">
         <v>100</v>
       </c>
@@ -12059,6 +12114,8 @@
       <c r="R42" s="23">
         <v>131</v>
       </c>
+      <c r="S42" s="30"/>
+      <c r="T42" s="30"/>
       <c r="U42" s="24">
         <v>100</v>
       </c>
@@ -12130,6 +12187,8 @@
       <c r="R43" s="23">
         <v>95</v>
       </c>
+      <c r="S43" s="30"/>
+      <c r="T43" s="30"/>
       <c r="U43" s="24">
         <v>100</v>
       </c>
@@ -12201,6 +12260,8 @@
       <c r="R44" s="23">
         <v>95</v>
       </c>
+      <c r="S44" s="30"/>
+      <c r="T44" s="30"/>
       <c r="U44" s="24">
         <v>100</v>
       </c>
@@ -12272,6 +12333,8 @@
       <c r="R45" s="23">
         <v>95</v>
       </c>
+      <c r="S45" s="30"/>
+      <c r="T45" s="30"/>
       <c r="U45" s="24">
         <v>100</v>
       </c>
@@ -12343,6 +12406,8 @@
       <c r="R46" s="23">
         <v>131</v>
       </c>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
       <c r="U46" s="24">
         <v>100</v>
       </c>
@@ -12414,6 +12479,8 @@
       <c r="R47" s="23">
         <v>131</v>
       </c>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
       <c r="U47" s="24">
         <v>100</v>
       </c>
@@ -12485,6 +12552,8 @@
       <c r="R48" s="23">
         <v>131</v>
       </c>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
       <c r="U48" s="24">
         <v>100</v>
       </c>
@@ -12556,6 +12625,8 @@
       <c r="R49" s="23">
         <v>131</v>
       </c>
+      <c r="S49" s="30"/>
+      <c r="T49" s="30"/>
       <c r="U49" s="24">
         <v>100</v>
       </c>
@@ -12627,6 +12698,8 @@
       <c r="R50" s="23">
         <v>131</v>
       </c>
+      <c r="S50" s="30"/>
+      <c r="T50" s="30"/>
       <c r="U50" s="24">
         <v>100</v>
       </c>
@@ -12698,6 +12771,8 @@
       <c r="R51" s="23">
         <v>131</v>
       </c>
+      <c r="S51" s="30"/>
+      <c r="T51" s="30"/>
       <c r="U51" s="24">
         <v>100</v>
       </c>
@@ -12769,6 +12844,8 @@
       <c r="R52" s="23">
         <v>131</v>
       </c>
+      <c r="S52" s="30"/>
+      <c r="T52" s="30"/>
       <c r="U52" s="24">
         <v>100</v>
       </c>
@@ -12840,6 +12917,8 @@
       <c r="R53" s="23">
         <v>131</v>
       </c>
+      <c r="S53" s="30"/>
+      <c r="T53" s="30"/>
       <c r="U53" s="24">
         <v>100</v>
       </c>
@@ -12911,6 +12990,8 @@
       <c r="R54" s="23">
         <v>131</v>
       </c>
+      <c r="S54" s="30"/>
+      <c r="T54" s="30"/>
       <c r="U54" s="24">
         <v>100</v>
       </c>
@@ -12982,6 +13063,8 @@
       <c r="R55" s="23">
         <v>131</v>
       </c>
+      <c r="S55" s="30"/>
+      <c r="T55" s="30"/>
       <c r="U55" s="24">
         <v>100</v>
       </c>
@@ -13053,6 +13136,8 @@
       <c r="R56" s="23">
         <v>131</v>
       </c>
+      <c r="S56" s="30"/>
+      <c r="T56" s="30"/>
       <c r="U56" s="24">
         <v>100</v>
       </c>
@@ -13124,6 +13209,8 @@
       <c r="R57" s="23">
         <v>131</v>
       </c>
+      <c r="S57" s="30"/>
+      <c r="T57" s="30"/>
       <c r="U57" s="24">
         <v>100</v>
       </c>
@@ -13195,6 +13282,8 @@
       <c r="R58" s="23">
         <v>131</v>
       </c>
+      <c r="S58" s="30"/>
+      <c r="T58" s="30"/>
       <c r="U58" s="24">
         <v>100</v>
       </c>
@@ -13266,6 +13355,8 @@
       <c r="R59" s="23">
         <v>95</v>
       </c>
+      <c r="S59" s="30"/>
+      <c r="T59" s="30"/>
       <c r="U59" s="24">
         <v>100</v>
       </c>
@@ -13337,6 +13428,8 @@
       <c r="R60" s="23">
         <v>131</v>
       </c>
+      <c r="S60" s="30"/>
+      <c r="T60" s="30"/>
       <c r="U60" s="24">
         <v>100</v>
       </c>
@@ -13408,6 +13501,8 @@
       <c r="R61" s="23">
         <v>95</v>
       </c>
+      <c r="S61" s="30"/>
+      <c r="T61" s="30"/>
       <c r="U61" s="24">
         <v>100</v>
       </c>
@@ -13479,6 +13574,8 @@
       <c r="R62" s="23">
         <v>95</v>
       </c>
+      <c r="S62" s="30"/>
+      <c r="T62" s="30"/>
       <c r="U62" s="24">
         <v>100</v>
       </c>
@@ -13550,6 +13647,8 @@
       <c r="R63" s="23">
         <v>95</v>
       </c>
+      <c r="S63" s="30"/>
+      <c r="T63" s="30"/>
       <c r="U63" s="24">
         <v>100</v>
       </c>
@@ -13621,6 +13720,8 @@
       <c r="R64" s="23">
         <v>95</v>
       </c>
+      <c r="S64" s="30"/>
+      <c r="T64" s="30"/>
       <c r="U64" s="24">
         <v>100</v>
       </c>
@@ -13692,6 +13793,8 @@
       <c r="R65" s="23">
         <v>95</v>
       </c>
+      <c r="S65" s="30"/>
+      <c r="T65" s="30"/>
       <c r="U65" s="24">
         <v>100</v>
       </c>
@@ -13763,6 +13866,8 @@
       <c r="R66" s="23">
         <v>95</v>
       </c>
+      <c r="S66" s="30"/>
+      <c r="T66" s="30"/>
       <c r="U66" s="24">
         <v>100</v>
       </c>
@@ -13834,6 +13939,8 @@
       <c r="R67" s="23">
         <v>95</v>
       </c>
+      <c r="S67" s="30"/>
+      <c r="T67" s="30"/>
       <c r="U67" s="24">
         <v>100</v>
       </c>
@@ -13905,6 +14012,8 @@
       <c r="R68" s="23">
         <v>131</v>
       </c>
+      <c r="S68" s="30"/>
+      <c r="T68" s="30"/>
       <c r="U68" s="24">
         <v>100</v>
       </c>
@@ -13976,6 +14085,8 @@
       <c r="R69" s="23">
         <v>131</v>
       </c>
+      <c r="S69" s="30"/>
+      <c r="T69" s="30"/>
       <c r="U69" s="24">
         <v>100</v>
       </c>
@@ -14047,6 +14158,8 @@
       <c r="R70" s="23">
         <v>131</v>
       </c>
+      <c r="S70" s="30"/>
+      <c r="T70" s="30"/>
       <c r="U70" s="24">
         <v>100</v>
       </c>
@@ -14118,6 +14231,8 @@
       <c r="R71" s="23">
         <v>131</v>
       </c>
+      <c r="S71" s="30"/>
+      <c r="T71" s="30"/>
       <c r="U71" s="24">
         <v>95</v>
       </c>
@@ -14189,6 +14304,8 @@
       <c r="R72" s="23">
         <v>131</v>
       </c>
+      <c r="S72" s="30"/>
+      <c r="T72" s="30"/>
       <c r="U72" s="24">
         <v>95</v>
       </c>
@@ -14260,6 +14377,8 @@
       <c r="R73" s="23">
         <v>125</v>
       </c>
+      <c r="S73" s="30"/>
+      <c r="T73" s="30"/>
       <c r="U73" s="24">
         <v>95</v>
       </c>
@@ -14331,6 +14450,8 @@
       <c r="R74" s="23">
         <v>125</v>
       </c>
+      <c r="S74" s="30"/>
+      <c r="T74" s="30"/>
       <c r="U74" s="24">
         <v>95</v>
       </c>
@@ -14402,6 +14523,8 @@
       <c r="R75" s="23">
         <v>125</v>
       </c>
+      <c r="S75" s="30"/>
+      <c r="T75" s="30"/>
       <c r="U75" s="24">
         <v>95</v>
       </c>
@@ -14473,6 +14596,8 @@
       <c r="R76" s="23">
         <v>131</v>
       </c>
+      <c r="S76" s="30"/>
+      <c r="T76" s="30"/>
       <c r="U76" s="24">
         <v>100</v>
       </c>
@@ -14544,6 +14669,8 @@
       <c r="R77" s="23">
         <v>131</v>
       </c>
+      <c r="S77" s="30"/>
+      <c r="T77" s="30"/>
       <c r="U77" s="24">
         <v>100</v>
       </c>
@@ -14615,6 +14742,8 @@
       <c r="R78" s="23">
         <v>131</v>
       </c>
+      <c r="S78" s="30"/>
+      <c r="T78" s="30"/>
       <c r="U78" s="24">
         <v>100</v>
       </c>
@@ -14686,6 +14815,8 @@
       <c r="R79" s="23">
         <v>131</v>
       </c>
+      <c r="S79" s="30"/>
+      <c r="T79" s="30"/>
       <c r="U79" s="24">
         <v>100</v>
       </c>
@@ -14757,6 +14888,8 @@
       <c r="R80" s="23">
         <v>131</v>
       </c>
+      <c r="S80" s="30"/>
+      <c r="T80" s="30"/>
       <c r="U80" s="24">
         <v>95</v>
       </c>
@@ -14828,6 +14961,8 @@
       <c r="R81" s="23">
         <v>131</v>
       </c>
+      <c r="S81" s="30"/>
+      <c r="T81" s="30"/>
       <c r="U81" s="24">
         <v>95</v>
       </c>
@@ -14899,6 +15034,8 @@
       <c r="R82" s="23">
         <v>131</v>
       </c>
+      <c r="S82" s="30"/>
+      <c r="T82" s="30"/>
       <c r="U82" s="24">
         <v>95</v>
       </c>
@@ -14970,6 +15107,8 @@
       <c r="R83" s="23">
         <v>131</v>
       </c>
+      <c r="S83" s="30"/>
+      <c r="T83" s="30"/>
       <c r="U83" s="24">
         <v>95</v>
       </c>
@@ -15041,6 +15180,8 @@
       <c r="R84" s="23">
         <v>131</v>
       </c>
+      <c r="S84" s="30"/>
+      <c r="T84" s="30"/>
       <c r="U84" s="24">
         <v>100</v>
       </c>
@@ -15112,6 +15253,8 @@
       <c r="R85" s="23">
         <v>131</v>
       </c>
+      <c r="S85" s="30"/>
+      <c r="T85" s="30"/>
       <c r="U85" s="24">
         <v>100</v>
       </c>
@@ -15183,6 +15326,8 @@
       <c r="R86" s="23">
         <v>125</v>
       </c>
+      <c r="S86" s="30"/>
+      <c r="T86" s="30"/>
       <c r="U86" s="24">
         <v>95</v>
       </c>
@@ -15254,6 +15399,8 @@
       <c r="R87" s="23">
         <v>125</v>
       </c>
+      <c r="S87" s="30"/>
+      <c r="T87" s="30"/>
       <c r="U87" s="24">
         <v>95</v>
       </c>
@@ -15325,6 +15472,8 @@
       <c r="R88" s="23">
         <v>125</v>
       </c>
+      <c r="S88" s="30"/>
+      <c r="T88" s="30"/>
       <c r="U88" s="24">
         <v>95</v>
       </c>
@@ -15396,6 +15545,8 @@
       <c r="R89" s="23">
         <v>125</v>
       </c>
+      <c r="S89" s="30"/>
+      <c r="T89" s="30"/>
       <c r="U89" s="24">
         <v>95</v>
       </c>
@@ -15467,6 +15618,8 @@
       <c r="R90" s="23">
         <v>125</v>
       </c>
+      <c r="S90" s="30"/>
+      <c r="T90" s="30"/>
       <c r="U90" s="24">
         <v>95</v>
       </c>
@@ -15538,6 +15691,8 @@
       <c r="R91" s="23">
         <v>131</v>
       </c>
+      <c r="S91" s="30"/>
+      <c r="T91" s="30"/>
       <c r="U91" s="24">
         <v>95</v>
       </c>
@@ -15609,6 +15764,8 @@
       <c r="R92" s="23">
         <v>131</v>
       </c>
+      <c r="S92" s="30"/>
+      <c r="T92" s="30"/>
       <c r="U92" s="24">
         <v>95</v>
       </c>
@@ -15680,6 +15837,8 @@
       <c r="R93" s="23">
         <v>131</v>
       </c>
+      <c r="S93" s="30"/>
+      <c r="T93" s="30"/>
       <c r="U93" s="24">
         <v>100</v>
       </c>
@@ -15905,6 +16064,8 @@
       <c r="R96" s="23">
         <v>131</v>
       </c>
+      <c r="S96" s="30"/>
+      <c r="T96" s="30"/>
       <c r="U96" s="24">
         <v>100</v>
       </c>
@@ -15976,6 +16137,8 @@
       <c r="R97" s="23">
         <v>131</v>
       </c>
+      <c r="S97" s="30"/>
+      <c r="T97" s="30"/>
       <c r="U97" s="24">
         <v>100</v>
       </c>
@@ -16047,6 +16210,8 @@
       <c r="R98" s="23">
         <v>131</v>
       </c>
+      <c r="S98" s="30"/>
+      <c r="T98" s="30"/>
       <c r="U98" s="24">
         <v>100</v>
       </c>
@@ -16503,6 +16668,8 @@
       <c r="R104" s="23">
         <v>131</v>
       </c>
+      <c r="S104" s="30"/>
+      <c r="T104" s="30"/>
       <c r="U104" s="24">
         <v>100</v>
       </c>
@@ -17190,6 +17357,8 @@
       <c r="R113" s="23">
         <v>0</v>
       </c>
+      <c r="S113" s="30"/>
+      <c r="T113" s="30"/>
       <c r="U113" s="24">
         <v>40</v>
       </c>
@@ -17261,6 +17430,8 @@
       <c r="R114" s="23">
         <v>131</v>
       </c>
+      <c r="S114" s="30"/>
+      <c r="T114" s="30"/>
       <c r="U114" s="24">
         <v>100</v>
       </c>
@@ -17332,6 +17503,8 @@
       <c r="R115" s="23">
         <v>35</v>
       </c>
+      <c r="S115" s="30"/>
+      <c r="T115" s="30"/>
       <c r="U115" s="24">
         <v>45</v>
       </c>
@@ -18096,6 +18269,8 @@
       <c r="R125" s="23">
         <v>131</v>
       </c>
+      <c r="S125" s="30"/>
+      <c r="T125" s="30"/>
       <c r="U125" s="24">
         <v>100</v>
       </c>
@@ -18475,6 +18650,8 @@
       <c r="R130" s="23">
         <v>131</v>
       </c>
+      <c r="S130" s="30"/>
+      <c r="T130" s="30"/>
       <c r="U130" s="24">
         <v>100</v>
       </c>
@@ -18546,6 +18723,8 @@
       <c r="R131" s="23">
         <v>131</v>
       </c>
+      <c r="S131" s="30"/>
+      <c r="T131" s="30"/>
       <c r="U131" s="24">
         <v>100</v>
       </c>
@@ -18617,6 +18796,8 @@
       <c r="R132" s="23">
         <v>131</v>
       </c>
+      <c r="S132" s="30"/>
+      <c r="T132" s="30"/>
       <c r="U132" s="24">
         <v>100</v>
       </c>
@@ -18688,6 +18869,8 @@
       <c r="R133" s="23">
         <v>131</v>
       </c>
+      <c r="S133" s="30"/>
+      <c r="T133" s="30"/>
       <c r="U133" s="24">
         <v>100</v>
       </c>
@@ -18759,6 +18942,8 @@
       <c r="R134" s="23">
         <v>131</v>
       </c>
+      <c r="S134" s="30"/>
+      <c r="T134" s="30"/>
       <c r="U134" s="24">
         <v>100</v>
       </c>
@@ -18830,6 +19015,8 @@
       <c r="R135" s="23">
         <v>131</v>
       </c>
+      <c r="S135" s="30"/>
+      <c r="T135" s="30"/>
       <c r="U135" s="24">
         <v>100</v>
       </c>
@@ -18901,6 +19088,8 @@
       <c r="R136" s="23">
         <v>131</v>
       </c>
+      <c r="S136" s="30"/>
+      <c r="T136" s="30"/>
       <c r="U136" s="24">
         <v>100</v>
       </c>
@@ -18972,6 +19161,8 @@
       <c r="R137" s="23">
         <v>131</v>
       </c>
+      <c r="S137" s="30"/>
+      <c r="T137" s="30"/>
       <c r="U137" s="24">
         <v>100</v>
       </c>
@@ -19043,6 +19234,8 @@
       <c r="R138" s="23">
         <v>131</v>
       </c>
+      <c r="S138" s="30"/>
+      <c r="T138" s="30"/>
       <c r="U138" s="24">
         <v>100</v>
       </c>
@@ -19114,6 +19307,8 @@
       <c r="R139" s="23">
         <v>131</v>
       </c>
+      <c r="S139" s="30"/>
+      <c r="T139" s="30"/>
       <c r="U139" s="24">
         <v>100</v>
       </c>
@@ -19185,6 +19380,8 @@
       <c r="R140" s="23">
         <v>131</v>
       </c>
+      <c r="S140" s="30"/>
+      <c r="T140" s="30"/>
       <c r="U140" s="24">
         <v>100</v>
       </c>
@@ -19256,6 +19453,8 @@
       <c r="R141" s="23">
         <v>131</v>
       </c>
+      <c r="S141" s="30"/>
+      <c r="T141" s="30"/>
       <c r="U141" s="24">
         <v>100</v>
       </c>
@@ -19481,6 +19680,8 @@
       <c r="R144" s="23">
         <v>125</v>
       </c>
+      <c r="S144" s="30"/>
+      <c r="T144" s="30"/>
       <c r="U144" s="24">
         <v>95</v>
       </c>
@@ -19552,6 +19753,8 @@
       <c r="R145" s="23">
         <v>125</v>
       </c>
+      <c r="S145" s="30"/>
+      <c r="T145" s="30"/>
       <c r="U145" s="24">
         <v>95</v>
       </c>
@@ -19623,6 +19826,8 @@
       <c r="R146" s="23">
         <v>125</v>
       </c>
+      <c r="S146" s="30"/>
+      <c r="T146" s="30"/>
       <c r="U146" s="24">
         <v>95</v>
       </c>
@@ -19694,6 +19899,8 @@
       <c r="R147" s="23">
         <v>125</v>
       </c>
+      <c r="S147" s="30"/>
+      <c r="T147" s="30"/>
       <c r="U147" s="24">
         <v>95</v>
       </c>
@@ -21536,6 +21743,8 @@
       <c r="R171" s="23">
         <v>125</v>
       </c>
+      <c r="S171" s="30"/>
+      <c r="T171" s="30"/>
       <c r="U171" s="24">
         <v>100</v>
       </c>
@@ -21992,6 +22201,8 @@
       <c r="R177" s="23">
         <v>131</v>
       </c>
+      <c r="S177" s="30"/>
+      <c r="T177" s="30"/>
       <c r="U177" s="24">
         <v>100</v>
       </c>
@@ -22448,6 +22659,8 @@
       <c r="R183" s="23">
         <v>131</v>
       </c>
+      <c r="S183" s="30"/>
+      <c r="T183" s="30"/>
       <c r="U183" s="24">
         <v>100</v>
       </c>
@@ -22519,6 +22732,8 @@
       <c r="R184" s="23">
         <v>125</v>
       </c>
+      <c r="S184" s="30"/>
+      <c r="T184" s="30"/>
       <c r="U184" s="24">
         <v>95</v>
       </c>
@@ -22590,6 +22805,8 @@
       <c r="R185" s="23">
         <v>125</v>
       </c>
+      <c r="S185" s="30"/>
+      <c r="T185" s="30"/>
       <c r="U185" s="24">
         <v>95</v>
       </c>
@@ -22661,6 +22878,8 @@
       <c r="R186" s="23">
         <v>125</v>
       </c>
+      <c r="S186" s="30"/>
+      <c r="T186" s="30"/>
       <c r="U186" s="24">
         <v>95</v>
       </c>
@@ -22732,6 +22951,8 @@
       <c r="R187" s="23">
         <v>125</v>
       </c>
+      <c r="S187" s="30"/>
+      <c r="T187" s="30"/>
       <c r="U187" s="24">
         <v>95</v>
       </c>
@@ -22803,6 +23024,8 @@
       <c r="R188" s="23">
         <v>125</v>
       </c>
+      <c r="S188" s="30"/>
+      <c r="T188" s="30"/>
       <c r="U188" s="24">
         <v>95</v>
       </c>
@@ -23182,6 +23405,8 @@
       <c r="R193" s="23">
         <v>131</v>
       </c>
+      <c r="S193" s="30"/>
+      <c r="T193" s="30"/>
       <c r="U193" s="24">
         <v>100</v>
       </c>
@@ -23253,6 +23478,8 @@
       <c r="R194" s="23">
         <v>131</v>
       </c>
+      <c r="S194" s="30"/>
+      <c r="T194" s="30"/>
       <c r="U194" s="24">
         <v>100</v>
       </c>
@@ -23555,6 +23782,8 @@
       <c r="R198" s="23">
         <v>125</v>
       </c>
+      <c r="S198" s="30"/>
+      <c r="T198" s="30"/>
       <c r="U198" s="24">
         <v>95</v>
       </c>
@@ -23626,6 +23855,8 @@
       <c r="R199" s="23">
         <v>125</v>
       </c>
+      <c r="S199" s="30"/>
+      <c r="T199" s="30"/>
       <c r="U199" s="24">
         <v>95</v>
       </c>
@@ -23697,6 +23928,8 @@
       <c r="R200" s="23">
         <v>125</v>
       </c>
+      <c r="S200" s="30"/>
+      <c r="T200" s="30"/>
       <c r="U200" s="24">
         <v>95</v>
       </c>
@@ -23768,6 +24001,8 @@
       <c r="R201" s="23">
         <v>125</v>
       </c>
+      <c r="S201" s="30"/>
+      <c r="T201" s="30"/>
       <c r="U201" s="24">
         <v>95</v>
       </c>
@@ -23993,6 +24228,8 @@
       <c r="R204" s="23">
         <v>131</v>
       </c>
+      <c r="S204" s="30"/>
+      <c r="T204" s="30"/>
       <c r="U204" s="24">
         <v>100</v>
       </c>
@@ -24295,6 +24532,8 @@
       <c r="R208" s="23">
         <v>125</v>
       </c>
+      <c r="S208" s="30"/>
+      <c r="T208" s="30"/>
       <c r="U208" s="24">
         <v>95</v>
       </c>
@@ -24828,6 +25067,8 @@
       <c r="R215" s="23">
         <v>131</v>
       </c>
+      <c r="S215" s="30"/>
+      <c r="T215" s="30"/>
       <c r="U215" s="24">
         <v>100</v>
       </c>
@@ -24899,6 +25140,8 @@
       <c r="R216" s="23">
         <v>131</v>
       </c>
+      <c r="S216" s="30"/>
+      <c r="T216" s="30"/>
       <c r="U216" s="24">
         <v>100</v>
       </c>
@@ -24970,6 +25213,8 @@
       <c r="R217" s="23">
         <v>131</v>
       </c>
+      <c r="S217" s="30"/>
+      <c r="T217" s="30"/>
       <c r="U217" s="24">
         <v>100</v>
       </c>
@@ -25041,6 +25286,8 @@
       <c r="R218" s="23">
         <v>131</v>
       </c>
+      <c r="S218" s="30"/>
+      <c r="T218" s="30"/>
       <c r="U218" s="24">
         <v>100</v>
       </c>
@@ -26113,6 +26360,8 @@
       <c r="R232" s="23">
         <v>131</v>
       </c>
+      <c r="S232" s="30"/>
+      <c r="T232" s="30"/>
       <c r="U232" s="24">
         <v>95</v>
       </c>
@@ -26184,6 +26433,8 @@
       <c r="R233" s="23">
         <v>131</v>
       </c>
+      <c r="S233" s="30"/>
+      <c r="T233" s="30"/>
       <c r="U233" s="24">
         <v>95</v>
       </c>
@@ -26255,6 +26506,8 @@
       <c r="R234" s="23">
         <v>131</v>
       </c>
+      <c r="S234" s="30"/>
+      <c r="T234" s="30"/>
       <c r="U234" s="24">
         <v>95</v>
       </c>
@@ -26326,6 +26579,8 @@
       <c r="R235" s="23">
         <v>131</v>
       </c>
+      <c r="S235" s="30"/>
+      <c r="T235" s="30"/>
       <c r="U235" s="24">
         <v>95</v>
       </c>
@@ -27167,6 +27422,8 @@
       <c r="R246" s="23">
         <v>131</v>
       </c>
+      <c r="S246" s="30"/>
+      <c r="T246" s="30"/>
       <c r="U246" s="24">
         <v>95</v>
       </c>
@@ -27238,6 +27495,8 @@
       <c r="R247" s="23">
         <v>131</v>
       </c>
+      <c r="S247" s="30"/>
+      <c r="T247" s="30"/>
       <c r="U247" s="24">
         <v>95</v>
       </c>
@@ -27617,6 +27876,8 @@
       <c r="R252" s="23">
         <v>131</v>
       </c>
+      <c r="S252" s="30"/>
+      <c r="T252" s="30"/>
       <c r="U252" s="24">
         <v>100</v>
       </c>
@@ -27688,6 +27949,8 @@
       <c r="R253" s="23">
         <v>125</v>
       </c>
+      <c r="S253" s="30"/>
+      <c r="T253" s="30"/>
       <c r="U253" s="24">
         <v>95</v>
       </c>
@@ -27759,6 +28022,8 @@
       <c r="R254" s="23">
         <v>131</v>
       </c>
+      <c r="S254" s="30"/>
+      <c r="T254" s="30"/>
       <c r="U254" s="24">
         <v>100</v>
       </c>
@@ -28523,6 +28788,8 @@
       <c r="R264" s="23">
         <v>131</v>
       </c>
+      <c r="S264" s="30"/>
+      <c r="T264" s="30"/>
       <c r="U264" s="24">
         <v>100</v>
       </c>
@@ -28594,6 +28861,8 @@
       <c r="R265" s="23">
         <v>131</v>
       </c>
+      <c r="S265" s="30"/>
+      <c r="T265" s="30"/>
       <c r="U265" s="24">
         <v>100</v>
       </c>
@@ -28665,6 +28934,8 @@
       <c r="R266" s="23">
         <v>131</v>
       </c>
+      <c r="S266" s="30"/>
+      <c r="T266" s="30"/>
       <c r="U266" s="24">
         <v>100</v>
       </c>
@@ -28736,6 +29007,8 @@
       <c r="R267" s="23">
         <v>131</v>
       </c>
+      <c r="S267" s="30"/>
+      <c r="T267" s="30"/>
       <c r="U267" s="24">
         <v>100</v>
       </c>
@@ -28807,6 +29080,8 @@
       <c r="R268" s="23">
         <v>131</v>
       </c>
+      <c r="S268" s="30"/>
+      <c r="T268" s="30"/>
       <c r="U268" s="24">
         <v>100</v>
       </c>
@@ -28878,6 +29153,8 @@
       <c r="R269" s="23">
         <v>131</v>
       </c>
+      <c r="S269" s="30"/>
+      <c r="T269" s="30"/>
       <c r="U269" s="24">
         <v>100</v>
       </c>
@@ -28949,6 +29226,8 @@
       <c r="R270" s="23">
         <v>131</v>
       </c>
+      <c r="S270" s="30"/>
+      <c r="T270" s="30"/>
       <c r="U270" s="24">
         <v>100</v>
       </c>
@@ -29020,6 +29299,8 @@
       <c r="R271" s="23">
         <v>125</v>
       </c>
+      <c r="S271" s="30"/>
+      <c r="T271" s="30"/>
       <c r="U271" s="24">
         <v>95</v>
       </c>
@@ -29168,6 +29449,8 @@
       <c r="R273" s="23">
         <v>131</v>
       </c>
+      <c r="S273" s="30"/>
+      <c r="T273" s="30"/>
       <c r="U273" s="24">
         <v>100</v>
       </c>
@@ -29239,6 +29522,8 @@
       <c r="R274" s="23">
         <v>131</v>
       </c>
+      <c r="S274" s="30"/>
+      <c r="T274" s="30"/>
       <c r="U274" s="24">
         <v>100</v>
       </c>
@@ -29310,6 +29595,8 @@
       <c r="R275" s="23">
         <v>131</v>
       </c>
+      <c r="S275" s="30"/>
+      <c r="T275" s="30"/>
       <c r="U275" s="24">
         <v>100</v>
       </c>
@@ -29381,6 +29668,8 @@
       <c r="R276" s="23">
         <v>131</v>
       </c>
+      <c r="S276" s="30"/>
+      <c r="T276" s="30"/>
       <c r="U276" s="24">
         <v>100</v>
       </c>
@@ -30607,6 +30896,8 @@
       <c r="R292" s="23">
         <v>131</v>
       </c>
+      <c r="S292" s="30"/>
+      <c r="T292" s="30"/>
       <c r="U292" s="24">
         <v>95</v>
       </c>
@@ -30678,6 +30969,8 @@
       <c r="R293" s="23">
         <v>125</v>
       </c>
+      <c r="S293" s="30"/>
+      <c r="T293" s="30"/>
       <c r="U293" s="24">
         <v>95</v>
       </c>
@@ -30749,6 +31042,8 @@
       <c r="R294" s="23">
         <v>131</v>
       </c>
+      <c r="S294" s="30"/>
+      <c r="T294" s="30"/>
       <c r="U294" s="24">
         <v>95</v>
       </c>
@@ -30820,6 +31115,8 @@
       <c r="R295" s="23">
         <v>125</v>
       </c>
+      <c r="S295" s="30"/>
+      <c r="T295" s="30"/>
       <c r="U295" s="24">
         <v>95</v>
       </c>
@@ -30891,6 +31188,8 @@
       <c r="R296" s="23">
         <v>131</v>
       </c>
+      <c r="S296" s="30"/>
+      <c r="T296" s="30"/>
       <c r="U296" s="24">
         <v>100</v>
       </c>
@@ -30962,6 +31261,8 @@
       <c r="R297" s="23">
         <v>131</v>
       </c>
+      <c r="S297" s="30"/>
+      <c r="T297" s="30"/>
       <c r="U297" s="24">
         <v>100</v>
       </c>
@@ -31033,6 +31334,8 @@
       <c r="R298" s="23">
         <v>125</v>
       </c>
+      <c r="S298" s="30"/>
+      <c r="T298" s="30"/>
       <c r="U298" s="24">
         <v>95</v>
       </c>
@@ -31104,6 +31407,8 @@
       <c r="R299" s="23">
         <v>131</v>
       </c>
+      <c r="S299" s="30"/>
+      <c r="T299" s="30"/>
       <c r="U299" s="24">
         <v>100</v>
       </c>
@@ -31175,6 +31480,8 @@
       <c r="R300" s="23">
         <v>131</v>
       </c>
+      <c r="S300" s="30"/>
+      <c r="T300" s="30"/>
       <c r="U300" s="24">
         <v>100</v>
       </c>
@@ -31246,6 +31553,8 @@
       <c r="R301" s="23">
         <v>131</v>
       </c>
+      <c r="S301" s="30"/>
+      <c r="T301" s="30"/>
       <c r="U301" s="24">
         <v>100</v>
       </c>
@@ -31317,6 +31626,8 @@
       <c r="R302" s="23">
         <v>131</v>
       </c>
+      <c r="S302" s="30"/>
+      <c r="T302" s="30"/>
       <c r="U302" s="24">
         <v>100</v>
       </c>
@@ -31388,6 +31699,8 @@
       <c r="R303" s="23">
         <v>131</v>
       </c>
+      <c r="S303" s="30"/>
+      <c r="T303" s="30"/>
       <c r="U303" s="24">
         <v>100</v>
       </c>
@@ -31459,6 +31772,8 @@
       <c r="R304" s="23">
         <v>131</v>
       </c>
+      <c r="S304" s="30"/>
+      <c r="T304" s="30"/>
       <c r="U304" s="24">
         <v>100</v>
       </c>
@@ -31530,6 +31845,8 @@
       <c r="R305" s="23">
         <v>131</v>
       </c>
+      <c r="S305" s="30"/>
+      <c r="T305" s="30"/>
       <c r="U305" s="24">
         <v>100</v>
       </c>
@@ -31601,6 +31918,8 @@
       <c r="R306" s="23">
         <v>125</v>
       </c>
+      <c r="S306" s="30"/>
+      <c r="T306" s="30"/>
       <c r="U306" s="24">
         <v>95</v>
       </c>
@@ -31672,6 +31991,8 @@
       <c r="R307" s="23">
         <v>125</v>
       </c>
+      <c r="S307" s="30"/>
+      <c r="T307" s="30"/>
       <c r="U307" s="24">
         <v>95</v>
       </c>
@@ -31743,6 +32064,8 @@
       <c r="R308" s="23">
         <v>131</v>
       </c>
+      <c r="S308" s="30"/>
+      <c r="T308" s="30"/>
       <c r="U308" s="24">
         <v>100</v>
       </c>
@@ -31814,6 +32137,8 @@
       <c r="R309" s="23">
         <v>125</v>
       </c>
+      <c r="S309" s="30"/>
+      <c r="T309" s="30"/>
       <c r="U309" s="24">
         <v>95</v>
       </c>
@@ -31885,6 +32210,8 @@
       <c r="R310" s="23">
         <v>131</v>
       </c>
+      <c r="S310" s="30"/>
+      <c r="T310" s="30"/>
       <c r="U310" s="24">
         <v>100</v>
       </c>
@@ -31956,6 +32283,8 @@
       <c r="R311" s="23">
         <v>131</v>
       </c>
+      <c r="S311" s="30"/>
+      <c r="T311" s="30"/>
       <c r="U311" s="24">
         <v>100</v>
       </c>
@@ -32027,6 +32356,8 @@
       <c r="R312" s="23">
         <v>75</v>
       </c>
+      <c r="S312" s="30"/>
+      <c r="T312" s="30"/>
       <c r="U312" s="24">
         <v>100</v>
       </c>
@@ -32098,6 +32429,8 @@
       <c r="R313" s="23">
         <v>131</v>
       </c>
+      <c r="S313" s="30"/>
+      <c r="T313" s="30"/>
       <c r="U313" s="24">
         <v>100</v>
       </c>
@@ -32169,6 +32502,8 @@
       <c r="R314" s="23">
         <v>131</v>
       </c>
+      <c r="S314" s="30"/>
+      <c r="T314" s="30"/>
       <c r="U314" s="24">
         <v>100</v>
       </c>
@@ -32240,6 +32575,8 @@
       <c r="R315" s="23">
         <v>131</v>
       </c>
+      <c r="S315" s="30"/>
+      <c r="T315" s="30"/>
       <c r="U315" s="24">
         <v>100</v>
       </c>
@@ -32311,6 +32648,8 @@
       <c r="R316" s="23">
         <v>131</v>
       </c>
+      <c r="S316" s="30"/>
+      <c r="T316" s="30"/>
       <c r="U316" s="24">
         <v>100</v>
       </c>
@@ -32382,6 +32721,8 @@
       <c r="R317" s="23">
         <v>131</v>
       </c>
+      <c r="S317" s="30"/>
+      <c r="T317" s="30"/>
       <c r="U317" s="24">
         <v>100</v>
       </c>
@@ -32453,6 +32794,8 @@
       <c r="R318" s="23">
         <v>75</v>
       </c>
+      <c r="S318" s="30"/>
+      <c r="T318" s="30"/>
       <c r="U318" s="24">
         <v>100</v>
       </c>
@@ -32524,6 +32867,8 @@
       <c r="R319" s="23">
         <v>75</v>
       </c>
+      <c r="S319" s="30"/>
+      <c r="T319" s="30"/>
       <c r="U319" s="24">
         <v>100</v>
       </c>
@@ -32595,6 +32940,8 @@
       <c r="R320" s="23">
         <v>75</v>
       </c>
+      <c r="S320" s="30"/>
+      <c r="T320" s="30"/>
       <c r="U320" s="24">
         <v>100</v>
       </c>
@@ -32666,6 +33013,8 @@
       <c r="R321" s="23">
         <v>75</v>
       </c>
+      <c r="S321" s="30"/>
+      <c r="T321" s="30"/>
       <c r="U321" s="24">
         <v>100</v>
       </c>
@@ -32814,6 +33163,8 @@
       <c r="R323" s="23">
         <v>75</v>
       </c>
+      <c r="S323" s="30"/>
+      <c r="T323" s="30"/>
       <c r="U323" s="24">
         <v>100</v>
       </c>
@@ -32885,6 +33236,8 @@
       <c r="R324" s="23">
         <v>131</v>
       </c>
+      <c r="S324" s="30"/>
+      <c r="T324" s="30"/>
       <c r="U324" s="24">
         <v>100</v>
       </c>
@@ -32956,6 +33309,8 @@
       <c r="R325" s="23">
         <v>131</v>
       </c>
+      <c r="S325" s="30"/>
+      <c r="T325" s="30"/>
       <c r="U325" s="24">
         <v>100</v>
       </c>
@@ -33027,6 +33382,8 @@
       <c r="R326" s="23">
         <v>75</v>
       </c>
+      <c r="S326" s="30"/>
+      <c r="T326" s="30"/>
       <c r="U326" s="24">
         <v>100</v>
       </c>
@@ -33098,6 +33455,8 @@
       <c r="R327" s="23">
         <v>131</v>
       </c>
+      <c r="S327" s="30"/>
+      <c r="T327" s="30"/>
       <c r="U327" s="24">
         <v>100</v>
       </c>
@@ -33169,6 +33528,8 @@
       <c r="R328" s="23">
         <v>131</v>
       </c>
+      <c r="S328" s="30"/>
+      <c r="T328" s="30"/>
       <c r="U328" s="24">
         <v>100</v>
       </c>
@@ -33240,6 +33601,8 @@
       <c r="R329" s="23">
         <v>131</v>
       </c>
+      <c r="S329" s="30"/>
+      <c r="T329" s="30"/>
       <c r="U329" s="24">
         <v>100</v>
       </c>
@@ -33311,6 +33674,8 @@
       <c r="R330" s="23">
         <v>75</v>
       </c>
+      <c r="S330" s="30"/>
+      <c r="T330" s="30"/>
       <c r="U330" s="24">
         <v>100</v>
       </c>
@@ -33382,6 +33747,8 @@
       <c r="R331" s="23">
         <v>75</v>
       </c>
+      <c r="S331" s="30"/>
+      <c r="T331" s="30"/>
       <c r="U331" s="24">
         <v>100</v>
       </c>
@@ -33453,6 +33820,8 @@
       <c r="R332" s="23">
         <v>125</v>
       </c>
+      <c r="S332" s="30"/>
+      <c r="T332" s="30"/>
       <c r="U332" s="24">
         <v>95</v>
       </c>
@@ -33524,6 +33893,8 @@
       <c r="R333" s="23">
         <v>125</v>
       </c>
+      <c r="S333" s="30"/>
+      <c r="T333" s="30"/>
       <c r="U333" s="24">
         <v>95</v>
       </c>
@@ -33595,6 +33966,8 @@
       <c r="R334" s="23">
         <v>125</v>
       </c>
+      <c r="S334" s="30"/>
+      <c r="T334" s="30"/>
       <c r="U334" s="24">
         <v>95</v>
       </c>
@@ -33666,6 +34039,8 @@
       <c r="R335" s="23">
         <v>125</v>
       </c>
+      <c r="S335" s="30"/>
+      <c r="T335" s="30"/>
       <c r="U335" s="24">
         <v>95</v>
       </c>
@@ -33737,6 +34112,8 @@
       <c r="R336" s="23">
         <v>125</v>
       </c>
+      <c r="S336" s="30"/>
+      <c r="T336" s="30"/>
       <c r="U336" s="24">
         <v>95</v>
       </c>
@@ -33808,6 +34185,8 @@
       <c r="R337" s="23">
         <v>125</v>
       </c>
+      <c r="S337" s="30"/>
+      <c r="T337" s="30"/>
       <c r="U337" s="24">
         <v>95</v>
       </c>
@@ -33879,6 +34258,8 @@
       <c r="R338" s="23">
         <v>125</v>
       </c>
+      <c r="S338" s="30"/>
+      <c r="T338" s="30"/>
       <c r="U338" s="24">
         <v>100</v>
       </c>
@@ -33950,6 +34331,8 @@
       <c r="R339" s="23">
         <v>125</v>
       </c>
+      <c r="S339" s="30"/>
+      <c r="T339" s="30"/>
       <c r="U339" s="24">
         <v>95</v>
       </c>
@@ -34021,6 +34404,8 @@
       <c r="R340" s="23">
         <v>125</v>
       </c>
+      <c r="S340" s="30"/>
+      <c r="T340" s="30"/>
       <c r="U340" s="24">
         <v>95</v>
       </c>
@@ -34092,6 +34477,8 @@
       <c r="R341" s="23">
         <v>125</v>
       </c>
+      <c r="S341" s="30"/>
+      <c r="T341" s="30"/>
       <c r="U341" s="24">
         <v>95</v>
       </c>
@@ -34163,6 +34550,8 @@
       <c r="R342" s="23">
         <v>125</v>
       </c>
+      <c r="S342" s="30"/>
+      <c r="T342" s="30"/>
       <c r="U342" s="24">
         <v>95</v>
       </c>
@@ -34234,6 +34623,8 @@
       <c r="R343" s="23">
         <v>131</v>
       </c>
+      <c r="S343" s="30"/>
+      <c r="T343" s="30"/>
       <c r="U343" s="24">
         <v>100</v>
       </c>
@@ -34305,6 +34696,8 @@
       <c r="R344" s="23">
         <v>131</v>
       </c>
+      <c r="S344" s="30"/>
+      <c r="T344" s="30"/>
       <c r="U344" s="24">
         <v>100</v>
       </c>
@@ -34376,6 +34769,8 @@
       <c r="R345" s="23">
         <v>131</v>
       </c>
+      <c r="S345" s="30"/>
+      <c r="T345" s="30"/>
       <c r="U345" s="24">
         <v>100</v>
       </c>
@@ -34447,6 +34842,8 @@
       <c r="R346" s="23">
         <v>131</v>
       </c>
+      <c r="S346" s="30"/>
+      <c r="T346" s="30"/>
       <c r="U346" s="24">
         <v>100</v>
       </c>
@@ -34518,6 +34915,8 @@
       <c r="R347" s="23">
         <v>131</v>
       </c>
+      <c r="S347" s="30"/>
+      <c r="T347" s="30"/>
       <c r="U347" s="24">
         <v>100</v>
       </c>
@@ -34589,6 +34988,8 @@
       <c r="R348" s="23">
         <v>131</v>
       </c>
+      <c r="S348" s="30"/>
+      <c r="T348" s="30"/>
       <c r="U348" s="24">
         <v>100</v>
       </c>
@@ -34660,6 +35061,8 @@
       <c r="R349" s="23">
         <v>131</v>
       </c>
+      <c r="S349" s="30"/>
+      <c r="T349" s="30"/>
       <c r="U349" s="24">
         <v>100</v>
       </c>
@@ -35116,6 +35519,8 @@
       <c r="R355" s="23">
         <v>125</v>
       </c>
+      <c r="S355" s="30"/>
+      <c r="T355" s="30"/>
       <c r="U355" s="24">
         <v>95</v>
       </c>
@@ -35187,6 +35592,8 @@
       <c r="R356" s="23">
         <v>125</v>
       </c>
+      <c r="S356" s="30"/>
+      <c r="T356" s="30"/>
       <c r="U356" s="24">
         <v>95</v>
       </c>
@@ -37568,6 +37975,8 @@
       <c r="R387" s="23">
         <v>131</v>
       </c>
+      <c r="S387" s="30"/>
+      <c r="T387" s="30"/>
       <c r="U387" s="24">
         <v>100</v>
       </c>
@@ -37639,6 +38048,8 @@
       <c r="R388" s="23">
         <v>131</v>
       </c>
+      <c r="S388" s="30"/>
+      <c r="T388" s="30"/>
       <c r="U388" s="24">
         <v>100</v>
       </c>
@@ -37710,6 +38121,8 @@
       <c r="R389" s="23">
         <v>131</v>
       </c>
+      <c r="S389" s="30"/>
+      <c r="T389" s="30"/>
       <c r="U389" s="24">
         <v>100</v>
       </c>
@@ -37781,6 +38194,8 @@
       <c r="R390" s="23">
         <v>131</v>
       </c>
+      <c r="S390" s="30"/>
+      <c r="T390" s="30"/>
       <c r="U390" s="24">
         <v>100</v>
       </c>
@@ -37852,6 +38267,8 @@
       <c r="R391" s="23">
         <v>131</v>
       </c>
+      <c r="S391" s="30"/>
+      <c r="T391" s="30"/>
       <c r="U391" s="24">
         <v>100</v>
       </c>
@@ -38462,6 +38879,8 @@
       <c r="R399" s="23">
         <v>50</v>
       </c>
+      <c r="S399" s="30"/>
+      <c r="T399" s="30"/>
       <c r="U399" s="24">
         <v>65</v>
       </c>
@@ -38533,6 +38952,8 @@
       <c r="R400" s="23">
         <v>131</v>
       </c>
+      <c r="S400" s="30"/>
+      <c r="T400" s="30"/>
       <c r="U400" s="24">
         <v>100</v>
       </c>
@@ -38678,6 +39099,8 @@
       <c r="R402" s="23">
         <v>131</v>
       </c>
+      <c r="S402" s="30"/>
+      <c r="T402" s="30"/>
       <c r="U402" s="24">
         <v>100</v>
       </c>
@@ -38749,6 +39172,8 @@
       <c r="R403" s="23">
         <v>131</v>
       </c>
+      <c r="S403" s="30"/>
+      <c r="T403" s="30"/>
       <c r="U403" s="24">
         <v>100</v>
       </c>
@@ -39051,6 +39476,8 @@
       <c r="R407" s="23">
         <v>131</v>
       </c>
+      <c r="S407" s="30"/>
+      <c r="T407" s="30"/>
       <c r="U407" s="24">
         <v>95</v>
       </c>
@@ -39122,6 +39549,8 @@
       <c r="R408" s="23">
         <v>131</v>
       </c>
+      <c r="S408" s="30"/>
+      <c r="T408" s="30"/>
       <c r="U408" s="24">
         <v>95</v>
       </c>
@@ -39193,6 +39622,8 @@
       <c r="R409" s="23">
         <v>131</v>
       </c>
+      <c r="S409" s="30"/>
+      <c r="T409" s="30"/>
       <c r="U409" s="24">
         <v>100</v>
       </c>
@@ -39264,6 +39695,8 @@
       <c r="R410" s="23">
         <v>131</v>
       </c>
+      <c r="S410" s="30"/>
+      <c r="T410" s="30"/>
       <c r="U410" s="24">
         <v>100</v>
       </c>
@@ -39335,6 +39768,8 @@
       <c r="R411" s="23">
         <v>131</v>
       </c>
+      <c r="S411" s="30"/>
+      <c r="T411" s="30"/>
       <c r="U411" s="24">
         <v>100</v>
       </c>
@@ -39406,6 +39841,8 @@
       <c r="R412" s="23">
         <v>131</v>
       </c>
+      <c r="S412" s="30"/>
+      <c r="T412" s="30"/>
       <c r="U412" s="24">
         <v>100</v>
       </c>
@@ -39477,6 +39914,8 @@
       <c r="R413" s="23">
         <v>131</v>
       </c>
+      <c r="S413" s="30"/>
+      <c r="T413" s="30"/>
       <c r="U413" s="24">
         <v>100</v>
       </c>
@@ -39548,6 +39987,8 @@
       <c r="R414" s="23">
         <v>131</v>
       </c>
+      <c r="S414" s="30"/>
+      <c r="T414" s="30"/>
       <c r="U414" s="24">
         <v>100</v>
       </c>
@@ -39619,6 +40060,8 @@
       <c r="R415" s="23">
         <v>131</v>
       </c>
+      <c r="S415" s="30"/>
+      <c r="T415" s="30"/>
       <c r="U415" s="24">
         <v>100</v>
       </c>
@@ -39690,6 +40133,8 @@
       <c r="R416" s="23">
         <v>131</v>
       </c>
+      <c r="S416" s="30"/>
+      <c r="T416" s="30"/>
       <c r="U416" s="24">
         <v>100</v>
       </c>
@@ -39761,6 +40206,8 @@
       <c r="R417" s="23">
         <v>125</v>
       </c>
+      <c r="S417" s="30"/>
+      <c r="T417" s="30"/>
       <c r="U417" s="24">
         <v>100</v>
       </c>
@@ -39832,6 +40279,8 @@
       <c r="R418" s="23">
         <v>131</v>
       </c>
+      <c r="S418" s="30"/>
+      <c r="T418" s="30"/>
       <c r="U418" s="24">
         <v>100</v>
       </c>
@@ -39903,6 +40352,8 @@
       <c r="R419" s="23">
         <v>131</v>
       </c>
+      <c r="S419" s="30"/>
+      <c r="T419" s="30"/>
       <c r="U419" s="24">
         <v>100</v>
       </c>
@@ -40282,6 +40733,8 @@
       <c r="R424" s="23">
         <v>131</v>
       </c>
+      <c r="S424" s="30"/>
+      <c r="T424" s="30"/>
       <c r="U424" s="24">
         <v>100</v>
       </c>
@@ -40353,6 +40806,8 @@
       <c r="R425" s="23">
         <v>125</v>
       </c>
+      <c r="S425" s="30"/>
+      <c r="T425" s="30"/>
       <c r="U425" s="24">
         <v>95</v>
       </c>
@@ -41040,6 +41495,8 @@
       <c r="R434" s="23">
         <v>131</v>
       </c>
+      <c r="S434" s="30"/>
+      <c r="T434" s="30"/>
       <c r="U434" s="24">
         <v>95</v>
       </c>
@@ -41111,6 +41568,8 @@
       <c r="R435" s="23">
         <v>131</v>
       </c>
+      <c r="S435" s="30"/>
+      <c r="T435" s="30"/>
       <c r="U435" s="24">
         <v>95</v>
       </c>
@@ -41259,6 +41718,8 @@
       <c r="R437" s="23">
         <v>131</v>
       </c>
+      <c r="S437" s="30"/>
+      <c r="T437" s="30"/>
       <c r="U437" s="24">
         <v>100</v>
       </c>
@@ -41330,6 +41791,8 @@
       <c r="R438" s="23">
         <v>131</v>
       </c>
+      <c r="S438" s="30"/>
+      <c r="T438" s="30"/>
       <c r="U438" s="24">
         <v>100</v>
       </c>
@@ -41401,6 +41864,8 @@
       <c r="R439" s="23">
         <v>131</v>
       </c>
+      <c r="S439" s="30"/>
+      <c r="T439" s="30"/>
       <c r="U439" s="24">
         <v>100</v>
       </c>
@@ -41549,6 +42014,8 @@
       <c r="R441" s="23">
         <v>131</v>
       </c>
+      <c r="S441" s="30"/>
+      <c r="T441" s="30"/>
       <c r="U441" s="24">
         <v>100</v>
       </c>
@@ -41620,6 +42087,8 @@
       <c r="R442" s="23">
         <v>131</v>
       </c>
+      <c r="S442" s="30"/>
+      <c r="T442" s="30"/>
       <c r="U442" s="24">
         <v>100</v>
       </c>
@@ -41691,6 +42160,8 @@
       <c r="R443" s="23">
         <v>131</v>
       </c>
+      <c r="S443" s="30"/>
+      <c r="T443" s="30"/>
       <c r="U443" s="24">
         <v>100</v>
       </c>
@@ -41762,6 +42233,8 @@
       <c r="R444" s="23">
         <v>131</v>
       </c>
+      <c r="S444" s="30"/>
+      <c r="T444" s="30"/>
       <c r="U444" s="24">
         <v>100</v>
       </c>
@@ -41987,6 +42460,8 @@
       <c r="R447" s="23">
         <v>131</v>
       </c>
+      <c r="S447" s="30"/>
+      <c r="T447" s="30"/>
       <c r="U447" s="24">
         <v>100</v>
       </c>
@@ -42366,6 +42841,8 @@
       <c r="R452" s="23">
         <v>131</v>
       </c>
+      <c r="S452" s="30"/>
+      <c r="T452" s="30"/>
       <c r="U452" s="24">
         <v>100</v>
       </c>
@@ -42437,6 +42914,8 @@
       <c r="R453" s="23">
         <v>131</v>
       </c>
+      <c r="S453" s="30"/>
+      <c r="T453" s="30"/>
       <c r="U453" s="24">
         <v>100</v>
       </c>
@@ -42508,6 +42987,8 @@
       <c r="R454" s="23">
         <v>131</v>
       </c>
+      <c r="S454" s="30"/>
+      <c r="T454" s="30"/>
       <c r="U454" s="24">
         <v>100</v>
       </c>
@@ -42887,6 +43368,8 @@
       <c r="R459" s="23">
         <v>131</v>
       </c>
+      <c r="S459" s="30"/>
+      <c r="T459" s="30"/>
       <c r="U459" s="24">
         <v>100</v>
       </c>
@@ -42958,6 +43441,8 @@
       <c r="R460" s="23">
         <v>131</v>
       </c>
+      <c r="S460" s="30"/>
+      <c r="T460" s="30"/>
       <c r="U460" s="24">
         <v>100</v>
       </c>
@@ -43808,6 +44293,7 @@
       <c r="Y497" s="14"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Y461" xr:uid="{FB4716B9-5855-4A9D-A33D-E582871FB114}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Code for DCE MCARE
Updated Code for DCE MCARE
</commit_message>
<xml_diff>
--- a/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD.xlsx
+++ b/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Hub Latest Project\mratdd\cukesatdd\src\main\resources\database\PlanDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8EA350-0758-46AD-9E2B-129462DCA029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DA5063-D059-41B4-93F0-BE9F575CFFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
+    <workbookView xWindow="20" yWindow="30" windowWidth="19180" windowHeight="10170" tabRatio="670" activeTab="2" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
   </bookViews>
   <sheets>
     <sheet name="MAPD_SNP_DCE" sheetId="1" r:id="rId1"/>
@@ -8972,7 +8972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4716B9-5855-4A9D-A33D-E582871FB114}">
   <dimension ref="A1:Y497"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
@@ -48745,9 +48745,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D150B402-BA8E-4A98-8F02-52FA07D02190}">
   <dimension ref="A1:AF104"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -48791,7 +48791,7 @@
         <v>2316</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>2731</v>
+        <v>12</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>2732</v>

</xml_diff>

<commit_message>
Data Update for Lis Buydown Plan
Data Update for Lis Buydown Plan
</commit_message>
<xml_diff>
--- a/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD.xlsx
+++ b/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Hub Latest Project\mratdd\cukesatdd\src\main\resources\database\PlanDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DA5063-D059-41B4-93F0-BE9F575CFFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F500D596-45E9-426D-A61A-685D570E1197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="19180" windowHeight="10170" tabRatio="670" activeTab="2" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" activeTab="5" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
   </bookViews>
   <sheets>
     <sheet name="MAPD_SNP_DCE" sheetId="1" r:id="rId1"/>
@@ -48745,7 +48745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D150B402-BA8E-4A98-8F02-52FA07D02190}">
   <dimension ref="A1:AF104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
     </sheetView>
@@ -64599,11 +64599,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1917EEC0-EAB8-420F-888C-D555647067A6}">
   <dimension ref="A1:R75"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>